<commit_message>
#1281 Regenated xlsx via new render.py to make sure everything works as expected
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="26621325E40" lockStructure="1"/>
+  <workbookProtection workbookPassword="4F7B9401087" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -12451,7 +12451,7 @@
     </row>
     <row r="3000"/>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="26621325E40"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4F7B9401087"/>
   <mergeCells count="2999">
     <mergeCell ref="A1913:B1913"/>
     <mergeCell ref="A854:B854"/>
@@ -15454,10 +15454,10 @@
     <mergeCell ref="A1615:B1615"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation sqref="A4:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
+    <dataValidation sqref="A4:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
     </dataValidation>
-    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
1279 Regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="A1577AF5138" lockStructure="1"/>
+  <workbookProtection workbookPassword="278BB8C2FF28" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -9449,7 +9449,7 @@
       <c r="A2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A1577AF5138"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="278BB8C2FF28"/>
   <dataValidations count="1">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
@@ -9487,7 +9487,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A1577AF5138"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="278BB8C2FF28"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
1279 Added missing fixture data for SEFA
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="278BB8C2FF28" lockStructure="1"/>
+  <workbookProtection workbookPassword="27540C525E76" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -9449,7 +9449,7 @@
       <c r="A2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="278BB8C2FF28"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27540C525E76"/>
   <dataValidations count="1">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
@@ -9487,7 +9487,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="278BB8C2FF28"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27540C525E76"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
1279 Regenarated output file
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="27540C525E76" lockStructure="1"/>
+  <workbookProtection workbookPassword="4C807AFCCE97" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -9449,7 +9449,7 @@
       <c r="A2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27540C525E76"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4C807AFCCE97"/>
   <dataValidations count="1">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
@@ -9487,7 +9487,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27540C525E76"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="4C807AFCCE97"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
continue building out secondary auditors
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
+++ b/backend/schemas/output/excel/xlsx/additional-ueis-template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="A1577AF5138" lockStructure="1"/>
+  <workbookProtection workbookPassword="A4DFA9096E1" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -9449,7 +9449,7 @@
       <c r="A2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A1577AF5138"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A4DFA9096E1"/>
   <dataValidations count="1">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>
@@ -9487,7 +9487,7 @@
       <c r="A2" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A1577AF5138"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="A4DFA9096E1"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>